<commit_message>
Se actualiza documentacion, pruebas realizadas
</commit_message>
<xml_diff>
--- a/Documentos proyecto San Ambiente/Fase3/Logs de prueba/Logs de prueba.xlsx
+++ b/Documentos proyecto San Ambiente/Fase3/Logs de prueba/Logs de prueba.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SanAmbiente\Proyecto-Sanambiente\Documentos proyecto San Ambiente\Fase3\Logs de prueba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE12AC04-67FB-47F5-813F-3BEA8DC98361}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A66579-E8BF-48F7-B0C9-7C07F2710F25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{6EC6B603-0429-4310-B5ED-B98F61A6BD01}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Estado</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Crear estacion (Tabla Parametro)</t>
   </si>
   <si>
-    <t>Conectar con estacion</t>
-  </si>
-  <si>
     <t>Crear Rango</t>
   </si>
   <si>
@@ -79,6 +76,9 @@
   </si>
   <si>
     <t>PDTE</t>
+  </si>
+  <si>
+    <t>Conectar con estacion*</t>
   </si>
 </sst>
 </file>
@@ -199,6 +199,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -212,12 +218,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -537,7 +537,7 @@
   <dimension ref="D7:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,38 +547,38 @@
   </cols>
   <sheetData>
     <row r="7" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D7" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="10" t="s">
+      <c r="D7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="F7" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="G7" s="10"/>
+      <c r="G7" s="12"/>
     </row>
     <row r="8" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
       <c r="F8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="5" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="12"/>
+      <c r="E9" s="7"/>
       <c r="F9" s="1"/>
       <c r="G9" s="4"/>
     </row>
     <row r="10" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="12"/>
+      <c r="E10" s="7"/>
       <c r="F10" s="2"/>
       <c r="G10" s="4"/>
     </row>
@@ -588,76 +588,85 @@
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="1"/>
+      <c r="G11" s="4"/>
     </row>
     <row r="12" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="12"/>
+      <c r="E12" s="7"/>
       <c r="F12" s="2"/>
       <c r="G12" s="4"/>
     </row>
     <row r="13" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="12"/>
+      <c r="E13" s="7"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="G13" s="4"/>
     </row>
     <row r="14" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="12"/>
+      <c r="E14" s="7"/>
       <c r="F14" s="2"/>
       <c r="G14" s="4"/>
     </row>
     <row r="15" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="12"/>
-      <c r="F15" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G15" s="7"/>
+      <c r="G15" s="9"/>
     </row>
     <row r="16" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="12"/>
+      <c r="E16" s="7"/>
       <c r="F16" s="2"/>
       <c r="G16" s="4"/>
     </row>
     <row r="17" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="7"/>
+      <c r="F17" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="9"/>
+    </row>
+    <row r="18" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D18" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D18" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="12"/>
+      <c r="E18" s="7"/>
       <c r="F18" s="2"/>
       <c r="G18" s="4"/>
     </row>
     <row r="19" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D19" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="12"/>
+      <c r="D19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="7"/>
       <c r="F19" s="2"/>
       <c r="G19" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="14">
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="D7:E8"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="D14:E14"/>
@@ -665,12 +674,6 @@
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="D7:E8"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D12:E12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>